<commit_message>
Results of balanced data
</commit_message>
<xml_diff>
--- a/digit_diff_positive/Results/summary.xlsx
+++ b/digit_diff_positive/Results/summary.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\Group_Learning\digit_diff_positive\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74D69B4-875C-4087-BFF6-EF5B655905F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093032F9-287A-4496-9B32-BBC18A4BD5F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E8F39B52-AE46-48A7-B34F-320AC446577C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{E8F39B52-AE46-48A7-B34F-320AC446577C}"/>
   </bookViews>
   <sheets>
-    <sheet name="traing digit 1" sheetId="1" r:id="rId1"/>
+    <sheet name="traing digit 1_unbalanced" sheetId="1" r:id="rId1"/>
+    <sheet name="training digit 1_balanced" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
   <si>
     <t>test digit</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -449,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C07D8600-7F87-4917-A465-0130E516A0CC}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -711,4 +712,272 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FBCCC0C-983B-40CD-A781-0A829D8326DB}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>52.2</v>
+      </c>
+      <c r="C2">
+        <v>46</v>
+      </c>
+      <c r="D2">
+        <v>31.2</v>
+      </c>
+      <c r="E2">
+        <v>81.8</v>
+      </c>
+      <c r="F2">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="G2">
+        <f>AVERAGE(B2:F2)</f>
+        <v>57.359999999999992</v>
+      </c>
+      <c r="H2">
+        <f>STDEV(B2:F2)</f>
+        <v>21.035874120178622</v>
+      </c>
+      <c r="I2">
+        <v>98.8</v>
+      </c>
+      <c r="J2">
+        <v>96.6</v>
+      </c>
+      <c r="K2">
+        <v>99.6</v>
+      </c>
+      <c r="L2">
+        <v>90.4</v>
+      </c>
+      <c r="M2">
+        <v>90.8</v>
+      </c>
+      <c r="N2">
+        <f>AVERAGE(I2:M2)</f>
+        <v>95.24</v>
+      </c>
+      <c r="O2">
+        <f>STDEV(I2:M2)</f>
+        <v>4.3781274536038772</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C3">
+        <v>0.4</v>
+      </c>
+      <c r="D3">
+        <v>0.4</v>
+      </c>
+      <c r="E3">
+        <v>14.4</v>
+      </c>
+      <c r="F3">
+        <v>0.4</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G5" si="0">AVERAGE(B3:F3)</f>
+        <v>3.5599999999999996</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H5" si="1">STDEV(B3:F3)</f>
+        <v>6.1096644752392093</v>
+      </c>
+      <c r="I3">
+        <v>99.4</v>
+      </c>
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3">
+        <v>99.4</v>
+      </c>
+      <c r="L3">
+        <v>95.2</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:N5" si="2">AVERAGE(I3:M3)</f>
+        <v>98.8</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ref="O3:O5" si="3">STDEV(I3:M3)</f>
+        <v>2.03469899493758</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>3.2</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>4.2</v>
+      </c>
+      <c r="E4">
+        <v>24.8</v>
+      </c>
+      <c r="F4">
+        <v>26.8</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>11.84</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>12.847879202420918</v>
+      </c>
+      <c r="I4">
+        <v>99.6</v>
+      </c>
+      <c r="J4">
+        <v>98.4</v>
+      </c>
+      <c r="K4">
+        <v>98.6</v>
+      </c>
+      <c r="L4">
+        <v>93.8</v>
+      </c>
+      <c r="M4">
+        <v>98</v>
+      </c>
+      <c r="N4">
+        <f t="shared" si="2"/>
+        <v>97.68</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="3"/>
+        <v>2.2476654555338076</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>5.4</v>
+      </c>
+      <c r="D5">
+        <v>6.6</v>
+      </c>
+      <c r="E5">
+        <v>13.4</v>
+      </c>
+      <c r="F5">
+        <v>29.8</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="0"/>
+        <v>11.24</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>11.28751522701077</v>
+      </c>
+      <c r="I5">
+        <v>96.8</v>
+      </c>
+      <c r="J5">
+        <v>95.4</v>
+      </c>
+      <c r="K5">
+        <v>95</v>
+      </c>
+      <c r="L5">
+        <v>97.6</v>
+      </c>
+      <c r="M5">
+        <v>93.2</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="2"/>
+        <v>95.6</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>1.7029386365926369</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>